<commit_message>
rill-analysis: Liantiao for luopan. FIXME: linux http client url param
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -203,39 +203,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>yyyyMMdd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllPosition.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getProdlines.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getIndicatorsByProdId.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getShowType.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchTrendByCondition.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>posIdString</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>prodlineId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>indicatorId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>posIdString</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yyyyMMdd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getAllPosition.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getProdlines.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getIndicatorsByProdId.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getShowType.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchTByCondition.action</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -837,11 +837,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84025344"/>
-        <c:axId val="84026880"/>
+        <c:axId val="55986816"/>
+        <c:axId val="71422336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84025344"/>
+        <c:axId val="55986816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,14 +850,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84026880"/>
+        <c:crossAx val="71422336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84026880"/>
+        <c:axId val="71422336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,13 +866,14 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84025344"/>
+        <c:crossAx val="55986816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -883,7 +884,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1229,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1445,7 +1446,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="16"/>
       <c r="G9" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1468,7 +1469,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
@@ -1476,7 +1477,7 @@
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" s="9"/>
     </row>
@@ -1485,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
@@ -1493,7 +1494,7 @@
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G12" s="9"/>
     </row>
@@ -1502,7 +1503,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
@@ -1513,7 +1514,7 @@
         <v>prodlineId</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G13" s="9"/>
     </row>
@@ -1531,7 +1532,7 @@
         <v>dateGranValue</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G14" s="15"/>
     </row>
@@ -1556,7 +1557,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1566,7 +1567,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1">

</xml_diff>

<commit_message>
rill-analysis: Add downloadFileName config support. Need change strategy of setWidgetAttribute in change event.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,6 +224,14 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}{1}{2}报表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>downloadFileName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,7 +498,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -562,6 +570,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -795,11 +806,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80617856"/>
-        <c:axId val="80619392"/>
+        <c:axId val="70797952"/>
+        <c:axId val="81449344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80617856"/>
+        <c:axId val="70797952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -808,14 +819,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80619392"/>
+        <c:crossAx val="81449344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80619392"/>
+        <c:axId val="81449344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +835,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80617856"/>
+        <c:crossAx val="70797952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -842,7 +853,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000666" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000666" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -884,8 +895,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G14" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A8:G14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G15" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A8:G15"/>
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
@@ -1217,13 +1228,13 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="25" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15">
@@ -1315,19 +1326,19 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="54" customHeight="1">
@@ -1496,6 +1507,22 @@
         <v>36</v>
       </c>
       <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="18" t="str">
+        <f>$B12&amp;" "&amp;$B13&amp;" "&amp;$B14</f>
+        <v>prodlineId indicatorId showFlag</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
rill-analysis: compatible enhancement for text/plain content-type but json content response
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
@@ -12,7 +12,7 @@
     <sheet name="_input" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="trendChartDataSource" localSheetId="2">OFFSET(_input!$A4,0,0,COUNTA(_input!$A:$A)-3, COUNTA(_input!$4:$4))</definedName>
+    <definedName name="trendChartDataSource" localSheetId="2">OFFSET(_input!$A5,0,0,COUNTA(_input!$A:$A)-4, COUNTA(_input!$5:$5))</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,6 +232,14 @@
   </si>
   <si>
     <t>downloadFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据粒度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按月查看</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -772,7 +780,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>_input!$A$5</c:f>
+              <c:f>_input!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -783,7 +791,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$B$4:$B$4</c:f>
+              <c:f>_input!$B$5:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -794,7 +802,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>_input!$B$5:$B$5</c:f>
+              <c:f>_input!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -806,11 +814,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="70797952"/>
-        <c:axId val="81449344"/>
+        <c:axId val="81403904"/>
+        <c:axId val="81405440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70797952"/>
+        <c:axId val="81403904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,14 +827,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81449344"/>
+        <c:crossAx val="81405440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81449344"/>
+        <c:axId val="81405440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +843,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70797952"/>
+        <c:crossAx val="81403904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -853,7 +861,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000711" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000711" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1229,8 +1237,8 @@
     </row>
     <row r="2" spans="2:15">
       <c r="B2" s="25" t="str">
-        <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
-        <v>搜索+推广点击消费趋势图</v>
+        <f>_input!$B2&amp;_input!$B3&amp;_input!$B4&amp;"报表"</f>
+        <v>搜索+推广点击消费按月查看报表</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -1543,7 +1551,7 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1566,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" customHeight="1" thickBot="1">
+    <row r="3" spans="1:2" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1574,19 +1582,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.25" thickBot="1">
+    <row r="4" spans="1:2" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>3344110</v>
       </c>
     </row>

</xml_diff>